<commit_message>
Signed-off-by: Jéfferson Pimenta Melo <jefferson.pimenta@hotmail.com>
</commit_message>
<xml_diff>
--- a/Aterramento_malha.xlsx
+++ b/Aterramento_malha.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="156">
   <si>
     <t>Espaçamento</t>
   </si>
@@ -245,9 +245,6 @@
     <t>Icft</t>
   </si>
   <si>
-    <t>Corrente de falta fase-terra sem envolver diretamente nenhum condutor de aterramento</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
@@ -444,6 +441,36 @@
   </si>
   <si>
     <t>Tensão de toque menor que a máxima tensão de toque</t>
+  </si>
+  <si>
+    <t>Tensão na periferia menor que a tensão máxima de toque</t>
+  </si>
+  <si>
+    <t>MAMEDE FILHO, J. Instalações Elétricas Industriais – LTC – 9a ed., 2017</t>
+  </si>
+  <si>
+    <t>Unid</t>
+  </si>
+  <si>
+    <t>Portanto, dado os parâmetros mostrados neste memorial, as dimensões e arranjo da malha se mostram adequadas</t>
+  </si>
+  <si>
+    <t>Conforme ABNT NBR 7117-1</t>
+  </si>
+  <si>
+    <t>Sondagem Geoelétrica</t>
+  </si>
+  <si>
+    <t>Corrente de choque existente devido à tensão de passo, com brita, na periferia da malha</t>
+  </si>
+  <si>
+    <t>Corrente de choque existente devido à tensão de passo, sem brita, na periferia da malha</t>
+  </si>
+  <si>
+    <t>Ipmsb&lt;Ich</t>
+  </si>
+  <si>
+    <t>Ipmcb&lt;Ich</t>
   </si>
   <si>
     <r>
@@ -457,61 +484,41 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Ec&lt;Ete</t>
+      <t>Ec&lt;Etm</t>
     </r>
   </si>
   <si>
-    <t>Tensão na periferia menor que a tensão máxima de toque</t>
-  </si>
-  <si>
-    <t>MAMEDE FILHO, J. Instalações Elétricas Industriais – LTC – 9a ed., 2017</t>
-  </si>
-  <si>
-    <t>Unid</t>
-  </si>
-  <si>
-    <t>Razão Social:</t>
-  </si>
-  <si>
-    <t>CPF/CNPJ:</t>
-  </si>
-  <si>
-    <t>Portanto, dado os parâmetros mostrados neste memorial, as dimensões e arranjo da malha se mostram adequadas</t>
-  </si>
-  <si>
-    <t>Conforme ABNT NBR 7117-1</t>
-  </si>
-  <si>
-    <t>Sondagem Geoelétrica</t>
-  </si>
-  <si>
-    <t>Corrente de choque existente devido à tensão de passo, com brita, na periferia da malha</t>
-  </si>
-  <si>
-    <t>Corrente de choque existente devido à tensão de passo, sem brita, na periferia da malha</t>
-  </si>
-  <si>
-    <t>Ipmsb&lt;Ich</t>
-  </si>
-  <si>
-    <t>Ipmcb&lt;Ich</t>
-  </si>
-  <si>
-    <t>Itmsb&lt;ch</t>
-  </si>
-  <si>
-    <t>Itmcb&lt;ch</t>
+    <t>Itmsb&lt;Ich</t>
+  </si>
+  <si>
+    <t>Itmcb&lt;Ich</t>
+  </si>
+  <si>
+    <t>Cordoalha 50mm²</t>
+  </si>
+  <si>
+    <t>PARÂMETROS DE ENTRADA</t>
+  </si>
+  <si>
+    <t>PARÂMETROS CALCULADOS</t>
+  </si>
+  <si>
+    <t>Corrente de falta fase-terra</t>
+  </si>
+  <si>
+    <t>Conforme ABNT NBR 15751</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -554,19 +561,46 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
-      <color theme="1"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="8">
@@ -669,7 +703,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -692,7 +726,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -707,9 +740,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -733,11 +763,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -748,14 +775,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -766,28 +817,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -823,7 +869,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1948,12 +1993,12 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>190330</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>24149</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="511207" cy="344453"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="CaixaDeTexto 1"/>
@@ -2067,7 +2112,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="CaixaDeTexto 1"/>
@@ -2161,7 +2206,7 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>122902</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>21759</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2171380" cy="308290"/>
@@ -2484,7 +2529,7 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>185786</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>36859</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1942844" cy="283026"/>
@@ -2807,7 +2852,7 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>24401</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>62152</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2369272" cy="232500"/>
@@ -3146,7 +3191,7 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>60527</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>84578</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2275168" cy="246542"/>
@@ -3485,7 +3530,7 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>214008</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>11405</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1783374" cy="374141"/>
@@ -3842,7 +3887,7 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>435093</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>9811</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1314719" cy="389081"/>
@@ -4061,7 +4106,7 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>159983</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>71738</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1852690" cy="350224"/>
@@ -4354,7 +4399,7 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>115958</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>2</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1838738" cy="371384"/>
@@ -4573,7 +4618,7 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>213504</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>50714</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1741192" cy="318421"/>
@@ -4866,7 +4911,7 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>77856</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>505238</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="650114" cy="389081"/>
@@ -5046,7 +5091,7 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>147845</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>61497</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1873112" cy="350865"/>
@@ -5258,7 +5303,7 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>107674</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>124239</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1880152" cy="352276"/>
@@ -5527,7 +5572,7 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>82412</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>95870</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1897132" cy="346633"/>
@@ -5739,7 +5784,7 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>49282</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>54457</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2137327" cy="348044"/>
@@ -6002,7 +6047,7 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>194641</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1895262" cy="356188"/>
@@ -6357,7 +6402,7 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>604631</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>33544</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2209800" cy="350224"/>
@@ -6728,7 +6773,7 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>487845</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>36857</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1195071" cy="318421"/>
@@ -6998,7 +7043,7 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>71644</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>62740</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2026902" cy="242054"/>
@@ -7464,7 +7509,7 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>255932</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>350147</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1479571" cy="368371"/>
@@ -8139,33 +8184,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
-        <v>147</v>
-      </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
+      <c r="A1" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="21" t="s">
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="19" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="17"/>
+      <c r="A3" s="15"/>
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
@@ -8181,7 +8226,7 @@
       <c r="F3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="22"/>
+      <c r="G3" s="20"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
@@ -8391,33 +8436,33 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="19"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="16" t="s">
+      <c r="A15" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="21" t="s">
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="19" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="17"/>
+      <c r="A16" s="15"/>
       <c r="B16" s="1" t="s">
         <v>3</v>
       </c>
@@ -8433,7 +8478,7 @@
       <c r="F16" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G16" s="22"/>
+      <c r="G16" s="20"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
@@ -8706,29 +8751,29 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="19" t="s">
+      <c r="A27" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="B27" s="19"/>
-      <c r="C27" s="19"/>
-      <c r="D27" s="19"/>
-      <c r="E27" s="19"/>
-      <c r="F27" s="19"/>
+      <c r="B27" s="17"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="17"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="16" t="s">
+      <c r="A28" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="18" t="s">
+      <c r="B28" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="17"/>
+      <c r="A29" s="15"/>
       <c r="B29" s="1" t="s">
         <v>11</v>
       </c>
@@ -9260,10 +9305,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J60"/>
+  <dimension ref="A1:J59"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScale="115" zoomScaleNormal="100" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="A60" sqref="A60"/>
+      <selection activeCell="B17" sqref="B17:C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9276,1319 +9321,1319 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
-        <v>143</v>
-      </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
+      <c r="A1" s="43" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="44" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" s="44"/>
+      <c r="J1" s="45" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
-        <v>144</v>
-      </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
+      <c r="A2" s="40" t="s">
+        <v>152</v>
+      </c>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="42"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17">
+        <v>448</v>
+      </c>
+      <c r="I3" s="17"/>
+      <c r="J3" s="8" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="I4" s="19"/>
-      <c r="J4" s="14" t="s">
-        <v>142</v>
+        <v>85</v>
+      </c>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17">
+        <v>472</v>
+      </c>
+      <c r="I4" s="17"/>
+      <c r="J4" s="8" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="B5" s="19" t="s">
-        <v>146</v>
-      </c>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19" t="s">
+      <c r="A5" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="19">
-        <v>448</v>
-      </c>
-      <c r="I5" s="19"/>
-      <c r="J5" s="9" t="s">
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17">
+        <v>445</v>
+      </c>
+      <c r="I5" s="17"/>
+      <c r="J5" s="8" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="B6" s="19"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19" t="s">
-        <v>88</v>
-      </c>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19">
-        <v>472</v>
-      </c>
-      <c r="I6" s="19"/>
-      <c r="J6" s="9" t="s">
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17">
+        <v>3000</v>
+      </c>
+      <c r="I6" s="17"/>
+      <c r="J6" s="8" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="B7" s="19"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19">
-        <v>445</v>
-      </c>
-      <c r="I7" s="19"/>
-      <c r="J7" s="9" t="s">
-        <v>27</v>
+      <c r="A7" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="29" t="s">
+        <v>154</v>
+      </c>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="16">
+        <v>871</v>
+      </c>
+      <c r="I7" s="16"/>
+      <c r="J7" s="8" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="B8" s="19"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19" t="s">
-        <v>87</v>
-      </c>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="19">
-        <v>3000</v>
-      </c>
-      <c r="I8" s="19"/>
-      <c r="J8" s="9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="I8" s="17"/>
+      <c r="J8" s="8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="B9" s="19"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="36" t="s">
-        <v>72</v>
-      </c>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="18">
-        <v>871</v>
-      </c>
-      <c r="I9" s="18"/>
-      <c r="J9" s="9" t="s">
-        <v>73</v>
+        <v>46</v>
+      </c>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17">
+        <v>57</v>
+      </c>
+      <c r="I9" s="17"/>
+      <c r="J9" s="8" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B10" s="19"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="36" t="s">
-        <v>75</v>
-      </c>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
-      <c r="G10" s="36"/>
-      <c r="H10" s="19">
-        <v>0.5</v>
-      </c>
-      <c r="I10" s="19"/>
-      <c r="J10" s="9" t="s">
-        <v>76</v>
+        <v>47</v>
+      </c>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17">
+        <v>41</v>
+      </c>
+      <c r="I10" s="17"/>
+      <c r="J10" s="8" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B11" s="19"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="19">
-        <v>57</v>
-      </c>
-      <c r="I11" s="19"/>
-      <c r="J11" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="I11" s="17"/>
+      <c r="J11" s="8" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B12" s="19"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19">
-        <v>41</v>
-      </c>
-      <c r="I12" s="19"/>
-      <c r="J12" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="39">
+        <v>1.4330000000000001E-2</v>
+      </c>
+      <c r="I12" s="39"/>
+      <c r="J12" s="8" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B13" s="19"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="19">
-        <v>0.5</v>
-      </c>
-      <c r="I13" s="19"/>
-      <c r="J13" s="9" t="s">
+      <c r="A13" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="B13" s="31"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="31" t="s">
+        <v>120</v>
+      </c>
+      <c r="E13" s="33"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="32"/>
+      <c r="H13" s="31">
+        <v>12</v>
+      </c>
+      <c r="I13" s="32"/>
+      <c r="J13" s="8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="B14" s="31"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="31" t="s">
+        <v>116</v>
+      </c>
+      <c r="E14" s="33"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="31">
+        <v>3</v>
+      </c>
+      <c r="I14" s="32"/>
+      <c r="J14" s="8" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B14" s="19"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19" t="s">
-        <v>57</v>
-      </c>
-      <c r="E14" s="19"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="19">
-        <v>1.4330000000000001E-2</v>
-      </c>
-      <c r="I14" s="19"/>
-      <c r="J14" s="9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="B15" s="28"/>
-      <c r="C15" s="30"/>
-      <c r="D15" s="28" t="s">
-        <v>121</v>
+    <row r="15" spans="1:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="29" t="s">
+        <v>111</v>
       </c>
       <c r="E15" s="29"/>
       <c r="F15" s="29"/>
-      <c r="G15" s="30"/>
-      <c r="H15" s="28">
-        <v>12</v>
-      </c>
-      <c r="I15" s="30"/>
-      <c r="J15" s="9" t="s">
-        <v>122</v>
+      <c r="G15" s="29"/>
+      <c r="H15" s="16">
+        <v>5</v>
+      </c>
+      <c r="I15" s="16"/>
+      <c r="J15" s="8" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="B16" s="28"/>
-      <c r="C16" s="30"/>
-      <c r="D16" s="28" t="s">
-        <v>117</v>
-      </c>
-      <c r="E16" s="29"/>
-      <c r="F16" s="29"/>
-      <c r="G16" s="30"/>
-      <c r="H16" s="28">
-        <v>3</v>
-      </c>
-      <c r="I16" s="30"/>
-      <c r="J16" s="9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="B17" s="19"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="36" t="s">
-        <v>112</v>
-      </c>
-      <c r="E17" s="36"/>
-      <c r="F17" s="36"/>
-      <c r="G17" s="36"/>
-      <c r="H17" s="18">
-        <v>5</v>
-      </c>
-      <c r="I17" s="18"/>
-      <c r="J17" s="9" t="s">
-        <v>34</v>
+      <c r="A16" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17">
+        <v>1000</v>
+      </c>
+      <c r="I16" s="17"/>
+      <c r="J16" s="8" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17">
+        <v>18</v>
+      </c>
+      <c r="I17" s="17"/>
+      <c r="J17" s="6" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="B18" s="19"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19" t="s">
-        <v>107</v>
-      </c>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="19">
-        <v>1000</v>
-      </c>
-      <c r="I18" s="19"/>
-      <c r="J18" s="9" t="s">
-        <v>108</v>
+      <c r="A18" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="17">
+        <v>13</v>
+      </c>
+      <c r="I18" s="17"/>
+      <c r="J18" s="6" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="40" t="s">
+        <v>153</v>
+      </c>
+      <c r="B19" s="41"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="41"/>
+      <c r="F19" s="41"/>
+      <c r="G19" s="41"/>
+      <c r="H19" s="41"/>
+      <c r="I19" s="41"/>
+      <c r="J19" s="42"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B19" s="19" t="s">
+      <c r="B20" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19" t="s">
+      <c r="C20" s="17"/>
+      <c r="D20" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="19"/>
-      <c r="H19" s="19">
-        <f>H11*H12</f>
+      <c r="E20" s="17"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="17">
+        <f>H9*H10</f>
         <v>2337</v>
       </c>
-      <c r="I19" s="19"/>
-      <c r="J19" s="6" t="s">
+      <c r="I20" s="17"/>
+      <c r="J20" s="6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
+    <row r="21" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B20" s="19"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="18" t="s">
+      <c r="B21" s="17"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="39">
-        <f>SQRT(H19/PI())</f>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="30">
+        <f>SQRT(H20/PI())</f>
         <v>27.274350661592639</v>
       </c>
-      <c r="I20" s="39"/>
-      <c r="J20" s="9" t="s">
+      <c r="I21" s="30"/>
+      <c r="J21" s="8" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B21" s="19"/>
-      <c r="C21" s="19"/>
-      <c r="D21" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="E21" s="19"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="19"/>
-      <c r="H21" s="19">
-        <v>18</v>
-      </c>
-      <c r="I21" s="19"/>
-      <c r="J21" s="6" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B22" s="19"/>
-      <c r="C22" s="19"/>
-      <c r="D22" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="E22" s="19"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="19">
-        <v>13</v>
-      </c>
-      <c r="I22" s="19"/>
+        <v>49</v>
+      </c>
+      <c r="B22" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="25">
+        <f>H9/H17</f>
+        <v>3.1666666666666665</v>
+      </c>
+      <c r="I22" s="25"/>
       <c r="J22" s="6" t="s">
-        <v>142</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B23" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="C23" s="19"/>
-      <c r="D23" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="E23" s="19"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="24">
-        <f>H11/H21</f>
-        <v>3.1666666666666665</v>
-      </c>
-      <c r="I23" s="24"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="25">
+        <f>H10/H18</f>
+        <v>3.1538461538461537</v>
+      </c>
+      <c r="I23" s="25"/>
       <c r="J23" s="6" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B24" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="C24" s="19"/>
-      <c r="D24" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="E24" s="19"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="24">
-        <f>H12/H22</f>
-        <v>3.1538461538461537</v>
-      </c>
-      <c r="I24" s="24"/>
+        <v>43</v>
+      </c>
+      <c r="B24" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" s="27"/>
+      <c r="D24" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="26">
+        <f>1.05*((H9*H18)+(H10*H17))</f>
+        <v>1552.95</v>
+      </c>
+      <c r="I24" s="26"/>
       <c r="J24" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B25" s="38" t="s">
-        <v>45</v>
-      </c>
-      <c r="C25" s="38"/>
-      <c r="D25" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
-      <c r="H25" s="35">
-        <f>1.05*((H11*H22)+(H12*H21))</f>
-        <v>1552.95</v>
-      </c>
-      <c r="I25" s="35"/>
-      <c r="J25" s="6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="B25" s="17"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="E25" s="27"/>
+      <c r="F25" s="27"/>
+      <c r="G25" s="27"/>
+      <c r="H25" s="30">
+        <f>(1/(2*PI()))*LN((H22^2)/(4*PI()*(H17-1)*H11*H12))</f>
+        <v>0.29915855647380496</v>
+      </c>
+      <c r="I25" s="30"/>
+      <c r="J25" s="6"/>
+    </row>
+    <row r="26" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="B26" s="19"/>
-      <c r="C26" s="19"/>
-      <c r="D26" s="38" t="s">
-        <v>48</v>
-      </c>
-      <c r="E26" s="38"/>
-      <c r="F26" s="38"/>
-      <c r="G26" s="38"/>
-      <c r="H26" s="39">
-        <f>(1/(2*PI()))*LN((H23^2)/(4*PI()*(H21-1)*H13*H14))</f>
-        <v>0.29915855647380496</v>
-      </c>
-      <c r="I26" s="39"/>
+        <v>60</v>
+      </c>
+      <c r="B26" s="17"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="E26" s="27"/>
+      <c r="F26" s="27"/>
+      <c r="G26" s="27"/>
+      <c r="H26" s="30">
+        <f>(1/(2*PI()))*LN((H23^2)/(4*PI()*(H18-1)*H11*H12))</f>
+        <v>0.3533019688108977</v>
+      </c>
+      <c r="I26" s="30"/>
       <c r="J26" s="6"/>
     </row>
-    <row r="27" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="B27" s="19"/>
-      <c r="C27" s="19"/>
-      <c r="D27" s="38" t="s">
-        <v>58</v>
-      </c>
-      <c r="E27" s="38"/>
-      <c r="F27" s="38"/>
-      <c r="G27" s="38"/>
-      <c r="H27" s="39">
-        <f>(1/(2*PI()))*LN((H24^2)/(4*PI()*(H22-1)*H13*H14))</f>
-        <v>0.3533019688108977</v>
-      </c>
-      <c r="I27" s="39"/>
+        <v>61</v>
+      </c>
+      <c r="B27" s="17"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="E27" s="27"/>
+      <c r="F27" s="27"/>
+      <c r="G27" s="27"/>
+      <c r="H27" s="28">
+        <f>(1/PI())*((1/(2*H11))+(1/(H22+H11))+(LN(0.655*(H17-1)-0.328)/H22^2))</f>
+        <v>0.48067573136695813</v>
+      </c>
+      <c r="I27" s="28"/>
       <c r="J27" s="6"/>
     </row>
-    <row r="28" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="38" t="s">
-        <v>62</v>
-      </c>
-      <c r="E28" s="38"/>
-      <c r="F28" s="38"/>
-      <c r="G28" s="38"/>
-      <c r="H28" s="40">
-        <f>(1/PI())*((1/(2*H13))+(1/(H23+H13))+(LN(0.655*(H21-1)-0.328)/H23^2))</f>
-        <v>0.48067573136695813</v>
-      </c>
-      <c r="I28" s="40"/>
+        <v>64</v>
+      </c>
+      <c r="B28" s="17"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="E28" s="27"/>
+      <c r="F28" s="27"/>
+      <c r="G28" s="27"/>
+      <c r="H28" s="28">
+        <f>(1/PI())*((1/(2*H11))+(1/(H23+H11))+(LN(0.655*(H18-1)-0.328)/H22^2))</f>
+        <v>0.46952011606323568</v>
+      </c>
+      <c r="I28" s="28"/>
       <c r="J28" s="6"/>
     </row>
-    <row r="29" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="B29" s="19"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="38" t="s">
-        <v>63</v>
-      </c>
-      <c r="E29" s="38"/>
-      <c r="F29" s="38"/>
-      <c r="G29" s="38"/>
-      <c r="H29" s="40">
-        <f>(1/PI())*((1/(2*H13))+(1/(H24+H13))+(LN(0.655*(H22-1)-0.328)/H23^2))</f>
-        <v>0.46952011606323568</v>
-      </c>
-      <c r="I29" s="40"/>
+        <v>66</v>
+      </c>
+      <c r="B29" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="C29" s="17"/>
+      <c r="D29" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="E29" s="17"/>
+      <c r="F29" s="17"/>
+      <c r="G29" s="17"/>
+      <c r="H29" s="17">
+        <f>0.65+0.172*H17</f>
+        <v>3.7459999999999996</v>
+      </c>
+      <c r="I29" s="17"/>
       <c r="J29" s="6"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="B30" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="C30" s="19"/>
-      <c r="D30" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="E30" s="19"/>
-      <c r="F30" s="19"/>
-      <c r="G30" s="19"/>
-      <c r="H30" s="19">
-        <f>0.65+0.172*H21</f>
-        <v>3.7459999999999996</v>
-      </c>
-      <c r="I30" s="19"/>
+        <v>77</v>
+      </c>
+      <c r="B30" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="C30" s="17"/>
+      <c r="D30" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="E30" s="17"/>
+      <c r="F30" s="17"/>
+      <c r="G30" s="17"/>
+      <c r="H30" s="17">
+        <f>0.65+0.172*H18</f>
+        <v>2.8859999999999997</v>
+      </c>
+      <c r="I30" s="17"/>
       <c r="J30" s="6"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="B31" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="B31" s="17"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="E31" s="27"/>
+      <c r="F31" s="27"/>
+      <c r="G31" s="27"/>
+      <c r="H31" s="26">
+        <f>MAX((H25*H29*H3*H7*SQRT(H8))/(0.116+0.174*H6),(H26*H30*H3*H7*SQRT(H8))/(0.116+0.174*H6))</f>
+        <v>592.22041051863675</v>
+      </c>
+      <c r="I31" s="26"/>
+      <c r="J31" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="C31" s="19"/>
-      <c r="D31" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="E31" s="19"/>
-      <c r="F31" s="19"/>
-      <c r="G31" s="19"/>
-      <c r="H31" s="19">
-        <f>0.65+0.172*H22</f>
-        <v>2.8859999999999997</v>
-      </c>
-      <c r="I31" s="19"/>
-      <c r="J31" s="6"/>
-    </row>
-    <row r="32" spans="1:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="B32" s="19"/>
-      <c r="C32" s="19"/>
-      <c r="D32" s="38" t="s">
-        <v>70</v>
-      </c>
-      <c r="E32" s="38"/>
-      <c r="F32" s="38"/>
-      <c r="G32" s="38"/>
-      <c r="H32" s="35">
-        <f>MAX((H26*H30*H5*H9*SQRT(H10))/(0.116+0.174*H8),(H27*H31*H5*H9*SQRT(H10))/(0.116+0.174*H8))</f>
-        <v>592.22041051863675</v>
-      </c>
-      <c r="I32" s="35"/>
+      <c r="B32" s="17"/>
+      <c r="C32" s="17"/>
+      <c r="D32" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="E32" s="16"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="16"/>
+      <c r="H32" s="26">
+        <f>(116+0.7*H6)/(SQRT(H8))</f>
+        <v>3133.8972542187785</v>
+      </c>
+      <c r="I32" s="26"/>
       <c r="J32" s="6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="B33" s="19"/>
-      <c r="C33" s="19"/>
-      <c r="D33" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="B33" s="17"/>
+      <c r="C33" s="17"/>
+      <c r="D33" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="E33" s="16"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="16"/>
+      <c r="H33" s="26">
+        <f>MAX((H27*H29*H4*H7)/(H24),(H28*H30*H4*H7)/(H24))</f>
+        <v>476.67530089919399</v>
+      </c>
+      <c r="I33" s="26"/>
+      <c r="J33" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="18"/>
-      <c r="H33" s="35">
-        <f>(116+0.7*H8)/(SQRT(H10))</f>
-        <v>3133.8972542187785</v>
-      </c>
-      <c r="I33" s="35"/>
-      <c r="J33" s="6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="B34" s="19"/>
-      <c r="C34" s="19"/>
-      <c r="D34" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="18"/>
-      <c r="H34" s="35">
-        <f>MAX((H28*H30*H6*H9)/(H25),(H29*H31*H6*H9)/(H25))</f>
-        <v>476.67530089919399</v>
-      </c>
-      <c r="I34" s="35"/>
+        <v>88</v>
+      </c>
+      <c r="B34" s="17"/>
+      <c r="C34" s="17"/>
+      <c r="D34" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="E34" s="16"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="16"/>
+      <c r="H34" s="26">
+        <f>(116+0.174*H6)/(SQRT(H8))</f>
+        <v>902.26825279403454</v>
+      </c>
+      <c r="I34" s="26"/>
       <c r="J34" s="6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="B35" s="19"/>
-      <c r="C35" s="19"/>
-      <c r="D35" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18"/>
-      <c r="G35" s="18"/>
-      <c r="H35" s="35">
-        <f>(116+0.174*H8)/(SQRT(H10))</f>
-        <v>902.26825279403454</v>
-      </c>
-      <c r="I35" s="35"/>
+      <c r="B35" s="17"/>
+      <c r="C35" s="17"/>
+      <c r="D35" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="E35" s="16"/>
+      <c r="F35" s="16"/>
+      <c r="G35" s="16"/>
+      <c r="H35" s="26">
+        <f>MAX((H25*H29*H4*H7)/(H24),(H26*H30*H4*H7)/(H24))</f>
+        <v>296.66880522173579</v>
+      </c>
+      <c r="I35" s="26"/>
       <c r="J35" s="6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="B36" s="19"/>
-      <c r="C36" s="19"/>
-      <c r="D36" s="18" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
-      <c r="G36" s="18"/>
-      <c r="H36" s="35">
-        <f>MAX((H26*H30*H6*H9)/(H25),(H27*H31*H6*H9)/(H25))</f>
-        <v>296.66880522173579</v>
-      </c>
-      <c r="I36" s="35"/>
-      <c r="J36" s="6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="17"/>
+      <c r="C36" s="17"/>
+      <c r="D36" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="E36" s="16"/>
+      <c r="F36" s="16"/>
+      <c r="G36" s="16"/>
+      <c r="H36" s="26">
+        <f>116/SQRT(H8)</f>
+        <v>164.04877323527901</v>
+      </c>
+      <c r="I36" s="26"/>
+      <c r="J36" s="7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="B37" s="19"/>
-      <c r="C37" s="19"/>
-      <c r="D37" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="B37" s="17"/>
+      <c r="C37" s="17"/>
+      <c r="D37" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="E37" s="27"/>
+      <c r="F37" s="27"/>
+      <c r="G37" s="27"/>
+      <c r="H37" s="26">
+        <f>(1000*H33)/(1000+6*H4)</f>
+        <v>124.39334574613622</v>
+      </c>
+      <c r="I37" s="26"/>
+      <c r="J37" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18"/>
-      <c r="G37" s="18"/>
-      <c r="H37" s="35">
-        <f>116/SQRT(H10)</f>
-        <v>164.04877323527901</v>
-      </c>
-      <c r="I37" s="35"/>
-      <c r="J37" s="7" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="B38" s="19"/>
-      <c r="C38" s="19"/>
-      <c r="D38" s="38" t="s">
         <v>97</v>
       </c>
-      <c r="E38" s="38"/>
-      <c r="F38" s="38"/>
-      <c r="G38" s="38"/>
-      <c r="H38" s="35">
-        <f>(1000*H34)/(1000+6*H6)</f>
-        <v>124.39334574613622</v>
-      </c>
-      <c r="I38" s="35"/>
+      <c r="B38" s="17"/>
+      <c r="C38" s="17"/>
+      <c r="D38" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="E38" s="27"/>
+      <c r="F38" s="27"/>
+      <c r="G38" s="27"/>
+      <c r="H38" s="26">
+        <f>(1000*H33)/(1000+6*(H4+H6))</f>
+        <v>21.83378989094879</v>
+      </c>
+      <c r="I38" s="26"/>
       <c r="J38" s="7" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="B39" s="19"/>
-      <c r="C39" s="19"/>
-      <c r="D39" s="38" t="s">
+        <v>100</v>
+      </c>
+      <c r="B39" s="17"/>
+      <c r="C39" s="17"/>
+      <c r="D39" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="E39" s="38"/>
-      <c r="F39" s="38"/>
-      <c r="G39" s="38"/>
-      <c r="H39" s="35">
-        <f>(1000*H34)/(1000+6*(H6+H8))</f>
-        <v>21.83378989094879</v>
-      </c>
-      <c r="I39" s="35"/>
+      <c r="E39" s="27"/>
+      <c r="F39" s="27"/>
+      <c r="G39" s="27"/>
+      <c r="H39" s="26">
+        <f>(1000*H35)/(1000+1.5*H4)</f>
+        <v>173.69367987221065</v>
+      </c>
+      <c r="I39" s="26"/>
       <c r="J39" s="7" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B40" s="17"/>
+      <c r="C40" s="17"/>
+      <c r="D40" s="27" t="s">
         <v>101</v>
       </c>
-      <c r="B40" s="19"/>
-      <c r="C40" s="19"/>
-      <c r="D40" s="38" t="s">
-        <v>100</v>
-      </c>
-      <c r="E40" s="38"/>
-      <c r="F40" s="38"/>
-      <c r="G40" s="38"/>
-      <c r="H40" s="35">
-        <f>(1000*H36)/(1000+1.5*H6)</f>
-        <v>173.69367987221065</v>
-      </c>
-      <c r="I40" s="35"/>
+      <c r="E40" s="27"/>
+      <c r="F40" s="27"/>
+      <c r="G40" s="27"/>
+      <c r="H40" s="26">
+        <f>(1000*H35)/(1000+1.5*(H4+H6))</f>
+        <v>47.788145171027026</v>
+      </c>
+      <c r="I40" s="26"/>
       <c r="J40" s="7" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="B41" s="19"/>
-      <c r="C41" s="19"/>
-      <c r="D41" s="38" t="s">
-        <v>102</v>
-      </c>
-      <c r="E41" s="38"/>
-      <c r="F41" s="38"/>
-      <c r="G41" s="38"/>
-      <c r="H41" s="35">
-        <f>(1000*H36)/(1000+1.5*(H6+H8))</f>
-        <v>47.788145171027026</v>
-      </c>
-      <c r="I41" s="35"/>
+      <c r="B41" s="17"/>
+      <c r="C41" s="17"/>
+      <c r="D41" s="27" t="s">
+        <v>104</v>
+      </c>
+      <c r="E41" s="27"/>
+      <c r="F41" s="27"/>
+      <c r="G41" s="27"/>
+      <c r="H41" s="26">
+        <f>((H16+1.5*H6)*9*H24)/(1000*H25*H29*H4)</f>
+        <v>145.3287276624026</v>
+      </c>
+      <c r="I41" s="26"/>
       <c r="J41" s="7" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="B42" s="19"/>
-      <c r="C42" s="19"/>
-      <c r="D42" s="38" t="s">
-        <v>105</v>
-      </c>
-      <c r="E42" s="38"/>
-      <c r="F42" s="38"/>
-      <c r="G42" s="38"/>
-      <c r="H42" s="35">
-        <f>((H18+1.5*H8)*9*H25)/(1000*H26*H30*H6)</f>
-        <v>145.3287276624026</v>
-      </c>
-      <c r="I42" s="35"/>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="B42" s="17"/>
+      <c r="C42" s="17"/>
+      <c r="D42" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="E42" s="16"/>
+      <c r="F42" s="16"/>
+      <c r="G42" s="16"/>
+      <c r="H42" s="26">
+        <f>(Auxiliar!D2-Auxiliar!E2)*((H4*H7)/(H31))</f>
+        <v>77.433303601438098</v>
+      </c>
+      <c r="I42" s="26"/>
       <c r="J42" s="7" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="B43" s="19"/>
-      <c r="C43" s="19"/>
-      <c r="D43" s="18" t="s">
-        <v>109</v>
-      </c>
-      <c r="E43" s="18"/>
-      <c r="F43" s="18"/>
-      <c r="G43" s="18"/>
-      <c r="H43" s="35">
-        <f>(Auxiliar!D2-Auxiliar!E2)*((H6*H9)/(H32))</f>
-        <v>77.433303601438098</v>
-      </c>
-      <c r="I43" s="35"/>
-      <c r="J43" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="B43" s="17"/>
+      <c r="C43" s="17"/>
+      <c r="D43" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="E43" s="16"/>
+      <c r="F43" s="16"/>
+      <c r="G43" s="16"/>
+      <c r="H43" s="26">
+        <f>((H5)/(4*H21))+(H5/H24)</f>
+        <v>4.3654752739182081</v>
+      </c>
+      <c r="I43" s="26"/>
+      <c r="J43" s="8" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="B44" s="19"/>
-      <c r="C44" s="19"/>
-      <c r="D44" s="18" t="s">
-        <v>114</v>
-      </c>
-      <c r="E44" s="18"/>
-      <c r="F44" s="18"/>
-      <c r="G44" s="18"/>
-      <c r="H44" s="35">
-        <f>((H7)/(4*H20))+(H7/H25)</f>
-        <v>4.3654752739182081</v>
-      </c>
-      <c r="I44" s="35"/>
-      <c r="J44" s="9" t="s">
-        <v>108</v>
+        <v>123</v>
+      </c>
+      <c r="B44" s="27" t="s">
+        <v>125</v>
+      </c>
+      <c r="C44" s="27"/>
+      <c r="D44" s="27" t="s">
+        <v>124</v>
+      </c>
+      <c r="E44" s="27"/>
+      <c r="F44" s="27"/>
+      <c r="G44" s="27"/>
+      <c r="H44" s="26">
+        <v>16.3</v>
+      </c>
+      <c r="I44" s="26"/>
+      <c r="J44" s="8" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="B45" s="38" t="s">
         <v>126</v>
       </c>
-      <c r="C45" s="38"/>
-      <c r="D45" s="38" t="s">
-        <v>125</v>
-      </c>
-      <c r="E45" s="38"/>
-      <c r="F45" s="38"/>
-      <c r="G45" s="38"/>
-      <c r="H45" s="35">
-        <v>16.3</v>
-      </c>
-      <c r="I45" s="35"/>
-      <c r="J45" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="17"/>
+      <c r="C45" s="17"/>
+      <c r="D45" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="E45" s="27"/>
+      <c r="F45" s="27"/>
+      <c r="G45" s="27"/>
+      <c r="H45" s="28">
+        <f>((H5)/(PI()*H24))*LN(((2*H24)/(H13*H14))+(((1.14125-0.0425*(H9/H10))*H24)/(SQRT(H20)))-(5.49-0.1443*(H9/H10))+1)</f>
+        <v>0.43417216817050425</v>
+      </c>
+      <c r="I45" s="28"/>
+      <c r="J45" s="8" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="B46" s="19"/>
-      <c r="C46" s="19"/>
-      <c r="D46" s="38" t="s">
         <v>128</v>
       </c>
-      <c r="E46" s="38"/>
-      <c r="F46" s="38"/>
-      <c r="G46" s="38"/>
-      <c r="H46" s="40">
-        <f>((H7)/(PI()*H25))*LN(((2*H25)/(H15*H16))+(((1.14125-0.0425*(H11/H12))*H25)/(SQRT(H19)))-(5.49-0.1443*(H11/H12))+1)</f>
-        <v>0.43417216817050425</v>
-      </c>
-      <c r="I46" s="40"/>
-      <c r="J46" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="7" t="s">
+      <c r="B46" s="17"/>
+      <c r="C46" s="17"/>
+      <c r="D46" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="B47" s="19"/>
-      <c r="C47" s="19"/>
-      <c r="D47" s="18" t="s">
+      <c r="E46" s="16"/>
+      <c r="F46" s="16"/>
+      <c r="G46" s="16"/>
+      <c r="H46" s="26">
+        <f>(H43*H44-H45^2)/(H43+H44-2*H45)</f>
+        <v>3.5847993184985305</v>
+      </c>
+      <c r="I46" s="26"/>
+      <c r="J46" s="8" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" s="35" t="s">
         <v>130</v>
       </c>
-      <c r="E47" s="18"/>
-      <c r="F47" s="18"/>
-      <c r="G47" s="18"/>
-      <c r="H47" s="35">
-        <f>(H44*H45-H46^2)/(H44+H45-2*H46)</f>
-        <v>3.5847993184985305</v>
-      </c>
+      <c r="B47" s="35"/>
+      <c r="C47" s="35"/>
+      <c r="D47" s="35"/>
+      <c r="E47" s="35"/>
+      <c r="F47" s="35"/>
+      <c r="G47" s="35"/>
+      <c r="H47" s="35"/>
       <c r="I47" s="35"/>
-      <c r="J47" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" s="37" t="s">
+      <c r="J47" s="35"/>
+    </row>
+    <row r="48" spans="1:10" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="22"/>
+      <c r="B48" s="23"/>
+      <c r="C48" s="23"/>
+      <c r="D48" s="23"/>
+      <c r="E48" s="23"/>
+      <c r="F48" s="23"/>
+      <c r="G48" s="23"/>
+      <c r="H48" s="23"/>
+      <c r="I48" s="23"/>
+      <c r="J48" s="24"/>
+    </row>
+    <row r="49" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A49" s="21" t="s">
         <v>131</v>
       </c>
-      <c r="B48" s="37"/>
-      <c r="C48" s="37"/>
-      <c r="D48" s="37"/>
-      <c r="E48" s="37"/>
-      <c r="F48" s="37"/>
-      <c r="G48" s="37"/>
-      <c r="H48" s="37"/>
-      <c r="I48" s="37"/>
-      <c r="J48" s="37"/>
-    </row>
-    <row r="49" spans="1:10" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="25"/>
-      <c r="B49" s="26"/>
-      <c r="C49" s="26"/>
-      <c r="D49" s="26"/>
-      <c r="E49" s="26"/>
-      <c r="F49" s="26"/>
-      <c r="G49" s="26"/>
-      <c r="H49" s="26"/>
-      <c r="I49" s="26"/>
-      <c r="J49" s="27"/>
-    </row>
-    <row r="50" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A50" s="41" t="s">
+      <c r="B49" s="21"/>
+      <c r="C49" s="21"/>
+      <c r="D49" s="21"/>
+      <c r="E49" s="21"/>
+      <c r="F49" s="21"/>
+      <c r="G49" s="21"/>
+      <c r="H49" s="21"/>
+      <c r="I49" s="21"/>
+      <c r="J49" s="21"/>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" s="31" t="s">
+        <v>135</v>
+      </c>
+      <c r="B50" s="33"/>
+      <c r="C50" s="33"/>
+      <c r="D50" s="33"/>
+      <c r="E50" s="33"/>
+      <c r="F50" s="32"/>
+      <c r="G50" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="H50" s="22" t="str">
+        <f>IF(H24&gt;H31,"Verdadeiro","Falso")</f>
+        <v>Verdadeiro</v>
+      </c>
+      <c r="I50" s="23"/>
+      <c r="J50" s="24"/>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51" s="31" t="s">
+        <v>136</v>
+      </c>
+      <c r="B51" s="33"/>
+      <c r="C51" s="33"/>
+      <c r="D51" s="33"/>
+      <c r="E51" s="33"/>
+      <c r="F51" s="32"/>
+      <c r="G51" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="B50" s="41"/>
-      <c r="C50" s="41"/>
-      <c r="D50" s="41"/>
-      <c r="E50" s="41"/>
-      <c r="F50" s="41"/>
-      <c r="G50" s="41"/>
-      <c r="H50" s="41"/>
-      <c r="I50" s="41"/>
-      <c r="J50" s="41"/>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A51" s="28" t="s">
-        <v>136</v>
-      </c>
-      <c r="B51" s="29"/>
-      <c r="C51" s="29"/>
-      <c r="D51" s="29"/>
-      <c r="E51" s="29"/>
-      <c r="F51" s="30"/>
-      <c r="G51" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="H51" s="25" t="str">
-        <f>IF(H25&gt;H32,"Verdadeiro","Falso")</f>
+      <c r="H51" s="22" t="str">
+        <f>IF(H32&gt;H33,"Verdadeiro","Falso")</f>
         <v>Verdadeiro</v>
       </c>
-      <c r="I51" s="26"/>
-      <c r="J51" s="27"/>
+      <c r="I51" s="23"/>
+      <c r="J51" s="24"/>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A52" s="28" t="s">
+      <c r="A52" s="31" t="s">
         <v>137</v>
       </c>
-      <c r="B52" s="29"/>
-      <c r="C52" s="29"/>
-      <c r="D52" s="29"/>
-      <c r="E52" s="29"/>
-      <c r="F52" s="30"/>
-      <c r="G52" s="12" t="s">
+      <c r="B52" s="33"/>
+      <c r="C52" s="33"/>
+      <c r="D52" s="33"/>
+      <c r="E52" s="33"/>
+      <c r="F52" s="32"/>
+      <c r="G52" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="H52" s="25" t="str">
-        <f>IF(H33&gt;H34,"Verdadeiro","Falso")</f>
+      <c r="H52" s="22" t="str">
+        <f>IF(H34&gt;H35,"Verdadeiro","Falso")</f>
         <v>Verdadeiro</v>
       </c>
-      <c r="I52" s="26"/>
-      <c r="J52" s="27"/>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A53" s="28" t="s">
+      <c r="I52" s="23"/>
+      <c r="J52" s="24"/>
+    </row>
+    <row r="53" spans="1:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="36" t="s">
+        <v>145</v>
+      </c>
+      <c r="B53" s="37"/>
+      <c r="C53" s="37"/>
+      <c r="D53" s="37"/>
+      <c r="E53" s="37"/>
+      <c r="F53" s="38"/>
+      <c r="G53" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="H53" s="22" t="str">
+        <f>IF(H37&lt;H36,"Verdadeiro","Falso")</f>
+        <v>Verdadeiro</v>
+      </c>
+      <c r="I53" s="23"/>
+      <c r="J53" s="24"/>
+    </row>
+    <row r="54" spans="1:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="36" t="s">
+        <v>144</v>
+      </c>
+      <c r="B54" s="37"/>
+      <c r="C54" s="37"/>
+      <c r="D54" s="37"/>
+      <c r="E54" s="37"/>
+      <c r="F54" s="38"/>
+      <c r="G54" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="H54" s="22" t="str">
+        <f>IF(H38&lt;H36,"Verdadeiro","Falso")</f>
+        <v>Verdadeiro</v>
+      </c>
+      <c r="I54" s="23"/>
+      <c r="J54" s="24"/>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="B55" s="23"/>
+      <c r="C55" s="23"/>
+      <c r="D55" s="23"/>
+      <c r="E55" s="23"/>
+      <c r="F55" s="24"/>
+      <c r="G55" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="H55" s="22" t="str">
+        <f>IF(H39&lt;H36,"Verdadeiro","Falso")</f>
+        <v>Falso</v>
+      </c>
+      <c r="I55" s="23"/>
+      <c r="J55" s="24"/>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="B56" s="23"/>
+      <c r="C56" s="23"/>
+      <c r="D56" s="23"/>
+      <c r="E56" s="23"/>
+      <c r="F56" s="24"/>
+      <c r="G56" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="H56" s="22" t="str">
+        <f>IF(H40&lt;H36,"Verdadeiro","Falso")</f>
+        <v>Verdadeiro</v>
+      </c>
+      <c r="I56" s="23"/>
+      <c r="J56" s="24"/>
+    </row>
+    <row r="57" spans="1:10" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A57" s="22" t="s">
         <v>138</v>
       </c>
-      <c r="B53" s="29"/>
-      <c r="C53" s="29"/>
-      <c r="D53" s="29"/>
-      <c r="E53" s="29"/>
-      <c r="F53" s="30"/>
-      <c r="G53" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="H53" s="25" t="str">
-        <f>IF(H35&gt;H36,"Verdadeiro","Falso")</f>
+      <c r="B57" s="23"/>
+      <c r="C57" s="23"/>
+      <c r="D57" s="23"/>
+      <c r="E57" s="23"/>
+      <c r="F57" s="24"/>
+      <c r="G57" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="H57" s="22" t="str">
+        <f>IF(H42&lt;H34,"Verdadeiro","Falso")</f>
         <v>Verdadeiro</v>
       </c>
-      <c r="I53" s="26"/>
-      <c r="J53" s="27"/>
-    </row>
-    <row r="54" spans="1:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="31" t="s">
-        <v>149</v>
-      </c>
-      <c r="B54" s="32"/>
-      <c r="C54" s="32"/>
-      <c r="D54" s="32"/>
-      <c r="E54" s="32"/>
-      <c r="F54" s="33"/>
-      <c r="G54" s="12" t="s">
-        <v>150</v>
-      </c>
-      <c r="H54" s="25" t="str">
-        <f>IF(H38&lt;H37,"Verdadeiro","Falso")</f>
-        <v>Verdadeiro</v>
-      </c>
-      <c r="I54" s="26"/>
-      <c r="J54" s="27"/>
-    </row>
-    <row r="55" spans="1:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="31" t="s">
-        <v>148</v>
-      </c>
-      <c r="B55" s="32"/>
-      <c r="C55" s="32"/>
-      <c r="D55" s="32"/>
-      <c r="E55" s="32"/>
-      <c r="F55" s="33"/>
-      <c r="G55" s="12" t="s">
-        <v>151</v>
-      </c>
-      <c r="H55" s="25" t="str">
-        <f>IF(H39&lt;H37,"Verdadeiro","Falso")</f>
-        <v>Verdadeiro</v>
-      </c>
-      <c r="I55" s="26"/>
-      <c r="J55" s="27"/>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A56" s="25" t="s">
-        <v>100</v>
-      </c>
-      <c r="B56" s="26"/>
-      <c r="C56" s="26"/>
-      <c r="D56" s="26"/>
-      <c r="E56" s="26"/>
-      <c r="F56" s="27"/>
-      <c r="G56" s="13" t="s">
-        <v>152</v>
-      </c>
-      <c r="H56" s="25" t="str">
-        <f>IF(H40&lt;H37,"Verdadeiro","Falso")</f>
-        <v>Falso</v>
-      </c>
-      <c r="I56" s="26"/>
-      <c r="J56" s="27"/>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A57" s="25" t="s">
-        <v>102</v>
-      </c>
-      <c r="B57" s="26"/>
-      <c r="C57" s="26"/>
-      <c r="D57" s="26"/>
-      <c r="E57" s="26"/>
-      <c r="F57" s="27"/>
-      <c r="G57" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="H57" s="25" t="str">
-        <f>IF(H41&lt;H38,"Verdadeiro","Falso")</f>
-        <v>Verdadeiro</v>
-      </c>
-      <c r="I57" s="26"/>
-      <c r="J57" s="27"/>
-    </row>
-    <row r="58" spans="1:10" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A58" s="25" t="s">
-        <v>140</v>
-      </c>
-      <c r="B58" s="26"/>
-      <c r="C58" s="26"/>
-      <c r="D58" s="26"/>
-      <c r="E58" s="26"/>
-      <c r="F58" s="27"/>
-      <c r="G58" s="12" t="s">
+      <c r="I57" s="23"/>
+      <c r="J57" s="24"/>
+    </row>
+    <row r="58" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="34" t="s">
+        <v>141</v>
+      </c>
+      <c r="B58" s="34"/>
+      <c r="C58" s="34"/>
+      <c r="D58" s="34"/>
+      <c r="E58" s="34"/>
+      <c r="F58" s="34"/>
+      <c r="G58" s="34"/>
+      <c r="H58" s="34"/>
+      <c r="I58" s="34"/>
+      <c r="J58" s="34"/>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59" s="13" t="s">
         <v>139</v>
-      </c>
-      <c r="H58" s="25" t="str">
-        <f>IF(H43&lt;H36,"Verdadeiro","Falso")</f>
-        <v>Verdadeiro</v>
-      </c>
-      <c r="I58" s="26"/>
-      <c r="J58" s="27"/>
-    </row>
-    <row r="59" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="34" t="s">
-        <v>145</v>
-      </c>
-      <c r="B59" s="34"/>
-      <c r="C59" s="34"/>
-      <c r="D59" s="34"/>
-      <c r="E59" s="34"/>
-      <c r="F59" s="34"/>
-      <c r="G59" s="34"/>
-      <c r="H59" s="34"/>
-      <c r="I59" s="34"/>
-      <c r="J59" s="34"/>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A60" s="15" t="s">
-        <v>141</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="154">
-    <mergeCell ref="A50:J50"/>
-    <mergeCell ref="A49:J49"/>
-    <mergeCell ref="H52:J52"/>
-    <mergeCell ref="H53:J53"/>
-    <mergeCell ref="H54:J54"/>
-    <mergeCell ref="H55:J55"/>
-    <mergeCell ref="A56:F56"/>
-    <mergeCell ref="H56:J56"/>
-    <mergeCell ref="A57:F57"/>
-    <mergeCell ref="H57:J57"/>
-    <mergeCell ref="D47:G47"/>
-    <mergeCell ref="H47:I47"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="D43:G43"/>
-    <mergeCell ref="H43:I43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="D44:G44"/>
-    <mergeCell ref="H44:I44"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="D46:G46"/>
-    <mergeCell ref="H46:I46"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="D24:G24"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="D33:G33"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D31:G31"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="D32:G32"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D29:G29"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="D34:G34"/>
     <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:G18"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:G17"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="D25:G25"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="D26:G26"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="D30:G30"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="D27:G27"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="D28:G28"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="D42:G42"/>
-    <mergeCell ref="H42:I42"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:G41"/>
-    <mergeCell ref="H41:I41"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="D20:G20"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:G19"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="D8:G8"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D15:G15"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="A59:J59"/>
-    <mergeCell ref="H51:J51"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="D35:G35"/>
-    <mergeCell ref="H35:I35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="D36:G36"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:G9"/>
+    <mergeCell ref="H9:I9"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="D10:G10"/>
     <mergeCell ref="H10:I10"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:G7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:G16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="A48:J48"/>
-    <mergeCell ref="H36:I36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:G23"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="H58:J58"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:G11"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="D18:G18"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:G12"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="D17:G17"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:G22"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="H57:J57"/>
+    <mergeCell ref="A50:F50"/>
     <mergeCell ref="A51:F51"/>
     <mergeCell ref="A52:F52"/>
     <mergeCell ref="A53:F53"/>
     <mergeCell ref="A54:F54"/>
-    <mergeCell ref="A55:F55"/>
-    <mergeCell ref="A58:F58"/>
+    <mergeCell ref="A57:F57"/>
+    <mergeCell ref="D37:G37"/>
+    <mergeCell ref="H37:I37"/>
+    <mergeCell ref="B38:C38"/>
     <mergeCell ref="D38:G38"/>
     <mergeCell ref="H38:I38"/>
     <mergeCell ref="B39:C39"/>
     <mergeCell ref="D39:G39"/>
     <mergeCell ref="H39:I39"/>
+    <mergeCell ref="D36:G36"/>
+    <mergeCell ref="H36:I36"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="A58:J58"/>
+    <mergeCell ref="H50:J50"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="D34:G34"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="D35:G35"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:G8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:G14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="A47:J47"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:G7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="D41:G41"/>
+    <mergeCell ref="H41:I41"/>
     <mergeCell ref="B40:C40"/>
     <mergeCell ref="D40:G40"/>
     <mergeCell ref="H40:I40"/>
-    <mergeCell ref="D37:G37"/>
-    <mergeCell ref="H37:I37"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="D46:G46"/>
+    <mergeCell ref="H46:I46"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:G42"/>
+    <mergeCell ref="H42:I42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="D43:G43"/>
+    <mergeCell ref="H43:I43"/>
     <mergeCell ref="B45:C45"/>
     <mergeCell ref="D45:G45"/>
     <mergeCell ref="H45:I45"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:G11"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D12:G12"/>
+    <mergeCell ref="D44:G44"/>
+    <mergeCell ref="H44:I44"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="D21:G21"/>
+    <mergeCell ref="H21:I21"/>
     <mergeCell ref="H12:I12"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:G20"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="H6:I6"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="D13:G13"/>
     <mergeCell ref="H13:I13"/>
-    <mergeCell ref="D22:G22"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="D14:G14"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="D21:G21"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:G9"/>
-    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A19:J19"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="D33:G33"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:G16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:G15"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D24:G24"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="D25:G25"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="D29:G29"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="D26:G26"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="D27:G27"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:G23"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="D32:G32"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="D30:G30"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D31:G31"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="D28:G28"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="A49:J49"/>
+    <mergeCell ref="A48:J48"/>
+    <mergeCell ref="H51:J51"/>
+    <mergeCell ref="H52:J52"/>
+    <mergeCell ref="H53:J53"/>
+    <mergeCell ref="H54:J54"/>
+    <mergeCell ref="A55:F55"/>
+    <mergeCell ref="H55:J55"/>
+    <mergeCell ref="A56:F56"/>
+    <mergeCell ref="H56:J56"/>
   </mergeCells>
   <pageMargins left="0.47101449275362317" right="0.45289855072463769" top="0.65217391304347827" bottom="0.61594202898550721" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="360" r:id="rId1"/>
-  <headerFooter>
-    <oddHeader>&amp;CMemória de Cálculo de Aterramento</oddHeader>
-    <oddFooter>&amp;RPágina &amp;P/&amp;N</oddFooter>
-  </headerFooter>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -10605,13 +10650,13 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E1" t="s">
         <v>118</v>
-      </c>
-      <c r="E1" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -10619,23 +10664,23 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <f>(A2*Memória!$H$23+Memória!$H$17)/(A2*Memória!$H$23)</f>
+        <f>(A2*Memória!$H$22+Memória!$H$15)/(A2*Memória!$H$22)</f>
         <v>1.7894736842105261</v>
       </c>
       <c r="C2">
-        <f>(A2*Memória!$H$23+(Memória!$H$17-1))/(A2*Memória!$H$23)</f>
+        <f>(A2*Memória!$H$22+(Memória!$H$15-1))/(A2*Memória!$H$22)</f>
         <v>1.631578947368421</v>
       </c>
       <c r="D2">
-        <f>(1/(2*PI()))*LN(((Memória!H13^2+Memória!H17^2)*(Memória!H13^2+(Memória!H23+Memória!H17)^2))/(Memória!H13*Memória!H14*(Memória!H10^2+Memória!H23^2)))+(1/PI())*LN(SUM(B2:B17))</f>
+        <f>(1/(2*PI()))*LN(((Memória!H11^2+Memória!H15^2)*(Memória!H11^2+(Memória!H22+Memória!H15)^2))/(Memória!H11*Memória!H12*(Memória!H8^2+Memória!H22^2)))+(1/PI())*LN(SUM(B2:B17))</f>
         <v>2.5493206987052583</v>
       </c>
       <c r="E2">
-        <f>(1/(2*PI()))*LN(((Memória!H13^2+(Memória!$H$17-1)^2)*(Memória!H13^2+(Memória!H23+(Memória!$H$17-1))^2))/(Memória!H13*Memória!H14*(Memória!H10^2+Memória!H23^2)))+(1/PI())*LN(SUM(B2:B17))</f>
+        <f>(1/(2*PI()))*LN(((Memória!H11^2+(Memória!$H$15-1)^2)*(Memória!H11^2+(Memória!H22+(Memória!$H$15-1))^2))/(Memória!H11*Memória!H12*(Memória!H8^2+Memória!H22^2)))+(1/PI())*LN(SUM(B2:B17))</f>
         <v>2.4377754680949675</v>
       </c>
       <c r="G2">
-        <f>Memória!H15</f>
+        <f>Memória!H13</f>
         <v>12</v>
       </c>
     </row>
@@ -10644,11 +10689,11 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <f>(A3*Memória!$H$23+Memória!$H$17)/(A3*Memória!$H$23)</f>
+        <f>(A3*Memória!$H$22+Memória!$H$15)/(A3*Memória!$H$22)</f>
         <v>1.5263157894736843</v>
       </c>
       <c r="C3">
-        <f>(A3*Memória!$H$23+(Memória!$H$17-1))/(A3*Memória!$H$23)</f>
+        <f>(A3*Memória!$H$22+(Memória!$H$15-1))/(A3*Memória!$H$22)</f>
         <v>1.4210526315789473</v>
       </c>
       <c r="G3">
@@ -10661,11 +10706,11 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <f>(A4*Memória!$H$23+Memória!$H$17)/(A4*Memória!$H$23)</f>
+        <f>(A4*Memória!$H$22+Memória!$H$15)/(A4*Memória!$H$22)</f>
         <v>1.3947368421052631</v>
       </c>
       <c r="C4">
-        <f>(A4*Memória!$H$23+(Memória!$H$17-1))/(A4*Memória!$H$23)</f>
+        <f>(A4*Memória!$H$22+(Memória!$H$15-1))/(A4*Memória!$H$22)</f>
         <v>1.3157894736842104</v>
       </c>
       <c r="G4">
@@ -10678,11 +10723,11 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <f>(A5*Memória!$H$23+Memória!$H$17)/(A5*Memória!$H$23)</f>
+        <f>(A5*Memória!$H$22+Memória!$H$15)/(A5*Memória!$H$22)</f>
         <v>1.3157894736842106</v>
       </c>
       <c r="C5">
-        <f>(A5*Memória!$H$23+(Memória!$H$17-1))/(A5*Memória!$H$23)</f>
+        <f>(A5*Memória!$H$22+(Memória!$H$15-1))/(A5*Memória!$H$22)</f>
         <v>1.2526315789473685</v>
       </c>
       <c r="G5">
@@ -10695,11 +10740,11 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <f>(A6*Memória!$H$23+Memória!$H$17)/(A6*Memória!$H$23)</f>
+        <f>(A6*Memória!$H$22+Memória!$H$15)/(A6*Memória!$H$22)</f>
         <v>1.263157894736842</v>
       </c>
       <c r="C6">
-        <f>(A6*Memória!$H$23+(Memória!$H$17-1))/(A6*Memória!$H$23)</f>
+        <f>(A6*Memória!$H$22+(Memória!$H$15-1))/(A6*Memória!$H$22)</f>
         <v>1.2105263157894737</v>
       </c>
       <c r="G6">
@@ -10712,11 +10757,11 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <f>(A7*Memória!$H$23+Memória!$H$17)/(A7*Memória!$H$23)</f>
+        <f>(A7*Memória!$H$22+Memória!$H$15)/(A7*Memória!$H$22)</f>
         <v>1.2255639097744362</v>
       </c>
       <c r="C7">
-        <f>(A7*Memória!$H$23+(Memória!$H$17-1))/(A7*Memória!$H$23)</f>
+        <f>(A7*Memória!$H$22+(Memória!$H$15-1))/(A7*Memória!$H$22)</f>
         <v>1.1804511278195489</v>
       </c>
       <c r="G7">
@@ -10729,11 +10774,11 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <f>(A8*Memória!$H$23+Memória!$H$17)/(A8*Memória!$H$23)</f>
+        <f>(A8*Memória!$H$22+Memória!$H$15)/(A8*Memória!$H$22)</f>
         <v>1.1973684210526316</v>
       </c>
       <c r="C8">
-        <f>(A8*Memória!$H$23+(Memória!$H$17-1))/(A8*Memória!$H$23)</f>
+        <f>(A8*Memória!$H$22+(Memória!$H$15-1))/(A8*Memória!$H$22)</f>
         <v>1.1578947368421053</v>
       </c>
       <c r="G8">
@@ -10746,11 +10791,11 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <f>(A9*Memória!$H$23+Memória!$H$17)/(A9*Memória!$H$23)</f>
+        <f>(A9*Memória!$H$22+Memória!$H$15)/(A9*Memória!$H$22)</f>
         <v>1.1754385964912282</v>
       </c>
       <c r="C9">
-        <f>(A9*Memória!$H$23+(Memória!$H$17-1))/(A9*Memória!$H$23)</f>
+        <f>(A9*Memória!$H$22+(Memória!$H$15-1))/(A9*Memória!$H$22)</f>
         <v>1.1403508771929824</v>
       </c>
       <c r="G9">
@@ -10763,11 +10808,11 @@
         <v>10</v>
       </c>
       <c r="B10">
-        <f>(A10*Memória!$H$23+Memória!$H$17)/(A10*Memória!$H$23)</f>
+        <f>(A10*Memória!$H$22+Memória!$H$15)/(A10*Memória!$H$22)</f>
         <v>1.1578947368421053</v>
       </c>
       <c r="C10">
-        <f>(A10*Memória!$H$23+(Memória!$H$17-1))/(A10*Memória!$H$23)</f>
+        <f>(A10*Memória!$H$22+(Memória!$H$15-1))/(A10*Memória!$H$22)</f>
         <v>1.1263157894736842</v>
       </c>
       <c r="G10">
@@ -10780,11 +10825,11 @@
         <v>11</v>
       </c>
       <c r="B11">
-        <f>(A11*Memória!$H$23+Memória!$H$17)/(A11*Memória!$H$23)</f>
+        <f>(A11*Memória!$H$22+Memória!$H$15)/(A11*Memória!$H$22)</f>
         <v>1.1435406698564594</v>
       </c>
       <c r="C11">
-        <f>(A11*Memória!$H$23+(Memória!$H$17-1))/(A11*Memória!$H$23)</f>
+        <f>(A11*Memória!$H$22+(Memória!$H$15-1))/(A11*Memória!$H$22)</f>
         <v>1.1148325358851674</v>
       </c>
       <c r="G11">
@@ -10797,11 +10842,11 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <f>(A12*Memória!$H$23+Memória!$H$17)/(A12*Memória!$H$23)</f>
+        <f>(A12*Memória!$H$22+Memória!$H$15)/(A12*Memória!$H$22)</f>
         <v>1.131578947368421</v>
       </c>
       <c r="C12">
-        <f>(A12*Memória!$H$23+(Memória!$H$17-1))/(A12*Memória!$H$23)</f>
+        <f>(A12*Memória!$H$22+(Memória!$H$15-1))/(A12*Memória!$H$22)</f>
         <v>1.1052631578947369</v>
       </c>
       <c r="G12">
@@ -10814,11 +10859,11 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <f>(A13*Memória!$H$23+Memória!$H$17)/(A13*Memória!$H$23)</f>
+        <f>(A13*Memória!$H$22+Memória!$H$15)/(A13*Memória!$H$22)</f>
         <v>1.1214574898785425</v>
       </c>
       <c r="C13">
-        <f>(A13*Memória!$H$23+(Memória!$H$17-1))/(A13*Memória!$H$23)</f>
+        <f>(A13*Memória!$H$22+(Memória!$H$15-1))/(A13*Memória!$H$22)</f>
         <v>1.097165991902834</v>
       </c>
     </row>
@@ -10827,11 +10872,11 @@
         <v>14</v>
       </c>
       <c r="B14">
-        <f>(A14*Memória!$H$23+Memória!$H$17)/(A14*Memória!$H$23)</f>
+        <f>(A14*Memória!$H$22+Memória!$H$15)/(A14*Memória!$H$22)</f>
         <v>1.112781954887218</v>
       </c>
       <c r="C14">
-        <f>(A14*Memória!$H$23+(Memória!$H$17-1))/(A14*Memória!$H$23)</f>
+        <f>(A14*Memória!$H$22+(Memória!$H$15-1))/(A14*Memória!$H$22)</f>
         <v>1.0902255639097744</v>
       </c>
     </row>
@@ -10840,11 +10885,11 @@
         <v>15</v>
       </c>
       <c r="B15">
-        <f>(A15*Memória!$H$23+Memória!$H$17)/(A15*Memória!$H$23)</f>
+        <f>(A15*Memória!$H$22+Memória!$H$15)/(A15*Memória!$H$22)</f>
         <v>1.1052631578947369</v>
       </c>
       <c r="C15">
-        <f>(A15*Memória!$H$23+(Memória!$H$17-1))/(A15*Memória!$H$23)</f>
+        <f>(A15*Memória!$H$22+(Memória!$H$15-1))/(A15*Memória!$H$22)</f>
         <v>1.0842105263157895</v>
       </c>
     </row>
@@ -10853,11 +10898,11 @@
         <v>16</v>
       </c>
       <c r="B16">
-        <f>(A16*Memória!$H$23+Memória!$H$17)/(A16*Memória!$H$23)</f>
+        <f>(A16*Memória!$H$22+Memória!$H$15)/(A16*Memória!$H$22)</f>
         <v>1.0986842105263157</v>
       </c>
       <c r="C16">
-        <f>(A16*Memória!$H$23+(Memória!$H$17-1))/(A16*Memória!$H$23)</f>
+        <f>(A16*Memória!$H$22+(Memória!$H$15-1))/(A16*Memória!$H$22)</f>
         <v>1.0789473684210527</v>
       </c>
     </row>
@@ -10866,11 +10911,11 @@
         <v>17</v>
       </c>
       <c r="B17">
-        <f>(A17*Memória!$H$23+Memória!$H$17)/(A17*Memória!$H$23)</f>
+        <f>(A17*Memória!$H$22+Memória!$H$15)/(A17*Memória!$H$22)</f>
         <v>1.0928792569659442</v>
       </c>
       <c r="C17">
-        <f>(A17*Memória!$H$23+(Memória!$H$17-1))/(A17*Memória!$H$23)</f>
+        <f>(A17*Memória!$H$22+(Memória!$H$15-1))/(A17*Memória!$H$22)</f>
         <v>1.0743034055727554</v>
       </c>
     </row>

</xml_diff>